<commit_message>
Add fritzing schematics and pinout datasheet
</commit_message>
<xml_diff>
--- a/doorbell-spy-BOM.xlsx
+++ b/doorbell-spy-BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Lab\automation\new-project-template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Lab\doorbell-spy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65DDF145-0969-454E-8D22-D602A1BF2867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{740E4062-67D3-47A4-A70D-5DCED03AEB27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>Quantity</t>
   </si>
@@ -64,6 +64,63 @@
   </si>
   <si>
     <t>Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raspberry Pi 3 Model B Vi. 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raspberry Pi </t>
+  </si>
+  <si>
+    <t>RASPBERRY PI 3</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>https://www.raspberrypi.com/products/raspberry-pi-3-model-b/</t>
+  </si>
+  <si>
+    <t>Raspberry Pi Camera Board v2 - 8 Megapixels</t>
+  </si>
+  <si>
+    <t>Adafruit</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/3099</t>
+  </si>
+  <si>
+    <t>Micro B USB Cable w/ LCD Voltage/Current Display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adafruit </t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/3388</t>
+  </si>
+  <si>
+    <t>USB WiFi Module</t>
+  </si>
+  <si>
+    <t>OURLink</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/1012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PIR Motion Sensor </t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/189</t>
+  </si>
+  <si>
+    <t>Micro SD Card - 16 GB - with adapter</t>
+  </si>
+  <si>
+    <t>Sandisk</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/2693</t>
   </si>
 </sst>
 </file>
@@ -157,7 +214,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -174,6 +231,22 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -457,23 +530,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L100"/>
+  <dimension ref="A1:L101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="22.5546875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
-    <col min="5" max="5" width="16.77734375" customWidth="1"/>
-    <col min="6" max="6" width="20.44140625" customWidth="1"/>
-    <col min="7" max="7" width="9" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="5"/>
+    <col min="2" max="2" width="44.109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" style="14" customWidth="1"/>
+    <col min="4" max="4" width="16" style="14" customWidth="1"/>
+    <col min="5" max="5" width="12" style="14" customWidth="1"/>
+    <col min="6" max="6" width="17.77734375" style="14" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" style="14" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="16"/>
     <col min="9" max="9" width="17.6640625" style="5" customWidth="1"/>
     <col min="10" max="10" width="35.5546875" style="3" customWidth="1"/>
     <col min="12" max="12" width="18.21875" customWidth="1"/>
@@ -484,22 +557,22 @@
       <c r="B1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="9" t="s">
+      <c r="G1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="13" t="s">
         <v>9</v>
       </c>
       <c r="I1" s="9" t="s">
@@ -512,54 +585,193 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H2" s="2"/>
+    <row r="2" spans="1:12" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="14">
+        <v>1</v>
+      </c>
+      <c r="H2" s="15">
+        <v>0</v>
+      </c>
       <c r="I2" s="2">
         <f>G2*H2</f>
         <v>0</v>
       </c>
+      <c r="J2" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="L2" s="5">
-        <f>SUM(I2:I50)</f>
-        <v>0</v>
+        <f>SUM(I2:I51)</f>
+        <v>83.75</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H3" s="2"/>
+      <c r="B3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="14">
+        <v>2693</v>
+      </c>
+      <c r="G3" s="14">
+        <v>1</v>
+      </c>
+      <c r="H3" s="15">
+        <v>19.95</v>
+      </c>
       <c r="I3" s="2">
-        <f t="shared" ref="I3:I66" si="0">G3*H3</f>
-        <v>0</v>
-      </c>
+        <f>G3*H3</f>
+        <v>19.95</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="5"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H4" s="2"/>
+      <c r="B4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="14">
+        <v>3099</v>
+      </c>
+      <c r="G4" s="14">
+        <v>1</v>
+      </c>
+      <c r="H4" s="15">
+        <v>29.95</v>
+      </c>
       <c r="I4" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="I4:I67" si="0">G4*H4</f>
+        <v>29.95</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H5" s="2"/>
+      <c r="B5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="14">
+        <v>3388</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="14">
+        <v>3388</v>
+      </c>
+      <c r="G5" s="14">
+        <v>1</v>
+      </c>
+      <c r="H5" s="15">
+        <v>9.9499999999999993</v>
+      </c>
       <c r="I5" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J5" s="4"/>
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H6" s="2"/>
+      <c r="B6" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="14">
+        <v>1012</v>
+      </c>
+      <c r="G6" s="14">
+        <v>1</v>
+      </c>
+      <c r="H6" s="15">
+        <v>13.95</v>
+      </c>
       <c r="I6" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>13.95</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H7" s="2"/>
+      <c r="B7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="14">
+        <v>189</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="14">
+        <v>189</v>
+      </c>
+      <c r="G7" s="14">
+        <v>1</v>
+      </c>
+      <c r="H7" s="15">
+        <v>9.9499999999999993</v>
+      </c>
       <c r="I7" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H8" s="15"/>
       <c r="I8" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -915,13 +1127,13 @@
     </row>
     <row r="67" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I67" s="2">
-        <f t="shared" ref="I67:I100" si="1">G67*H67</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I68" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="I68:I101" si="1">G68*H68</f>
         <v>0</v>
       </c>
     </row>
@@ -1113,6 +1325,12 @@
     </row>
     <row r="100" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I100" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I101" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>

</xml_diff>